<commit_message>
excel import and css tune up
</commit_message>
<xml_diff>
--- a/saibabacharityreceiptor/template.xlsx
+++ b/saibabacharityreceiptor/template.xlsx
@@ -16,55 +16,73 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Donation Amount</t>
+  </si>
+  <si>
+    <t>Donation Amount in Words</t>
+  </si>
+  <si>
+    <t>Merchandise Item</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Recurring Dates (with comma separated)</t>
+  </si>
+  <si>
+    <t>Receipt Type</t>
+  </si>
+  <si>
+    <t>Hours Served</t>
+  </si>
+  <si>
+    <t>Mode Of Payment</t>
+  </si>
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Contact</t>
-  </si>
-  <si>
-    <t>Donation Amount</t>
-  </si>
-  <si>
-    <t>Donation Amount in Words</t>
-  </si>
-  <si>
-    <t>Merchandise Item</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>HoursServed</t>
-  </si>
-  <si>
-    <t>Recurring Dates (with comma separated)</t>
-  </si>
-  <si>
-    <t>ModeOfPayment</t>
-  </si>
-  <si>
-    <t>ReceiptType</t>
+    <t>Received By</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -84,13 +102,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -383,68 +408,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="27" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1"/>
-    <col min="10" max="10" width="37.7109375" customWidth="1"/>
-    <col min="11" max="11" width="17.140625" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="27" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="37.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="D2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updated fields for excel import
</commit_message>
<xml_diff>
--- a/saibabacharityreceiptor/template.xlsx
+++ b/saibabacharityreceiptor/template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Address</t>
   </si>
@@ -51,10 +51,43 @@
     <t>Mode Of Payment</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Received By</t>
+  </si>
+  <si>
+    <t>Frist Name</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Zip Code</t>
+  </si>
+  <si>
+    <t>Date Received</t>
+  </si>
+  <si>
+    <t>Issued Date</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Service Type</t>
+  </si>
+  <si>
+    <t>Rate per hour</t>
+  </si>
+  <si>
+    <t>FMV Value</t>
   </si>
 </sst>
 </file>
@@ -408,71 +441,113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="27" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" customWidth="1"/>
-    <col min="11" max="11" width="37.7109375" customWidth="1"/>
-    <col min="12" max="12" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="6" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="7" width="6.42578125" customWidth="1"/>
+    <col min="8" max="8" width="9" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" customWidth="1"/>
+    <col min="14" max="14" width="25.28515625" customWidth="1"/>
+    <col min="15" max="15" width="37.7109375" customWidth="1"/>
+    <col min="16" max="16" width="17.28515625" customWidth="1"/>
+    <col min="17" max="17" width="10.28515625" customWidth="1"/>
+    <col min="18" max="18" width="7.28515625" customWidth="1"/>
+    <col min="19" max="19" width="12.42578125" customWidth="1"/>
+    <col min="20" max="22" width="12.85546875" customWidth="1"/>
+    <col min="23" max="23" width="17.140625" customWidth="1"/>
+    <col min="24" max="24" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1">
+    <row r="1" spans="1:24" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="2" spans="1:13">
-      <c r="D2" s="2"/>
+    <row r="2" spans="1:24">
+      <c r="I2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
improved css and excel download
</commit_message>
<xml_diff>
--- a/saibabacharityreceiptor/template.xlsx
+++ b/saibabacharityreceiptor/template.xlsx
@@ -72,12 +72,6 @@
     <t>Zip Code</t>
   </si>
   <si>
-    <t>Date Received</t>
-  </si>
-  <si>
-    <t>Issued Date</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -88,6 +82,12 @@
   </si>
   <si>
     <t>FMV Value</t>
+  </si>
+  <si>
+    <t>Date Received (mm/dd/yyyy)</t>
+  </si>
+  <si>
+    <t>Issued Date(mm/dd/yyyy)</t>
   </si>
 </sst>
 </file>
@@ -443,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -458,8 +458,8 @@
     <col min="8" max="8" width="9" customWidth="1"/>
     <col min="9" max="9" width="6.28515625" customWidth="1"/>
     <col min="10" max="10" width="8.28515625" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" customWidth="1"/>
-    <col min="12" max="12" width="11" customWidth="1"/>
+    <col min="11" max="11" width="25.5703125" customWidth="1"/>
+    <col min="12" max="12" width="21" customWidth="1"/>
     <col min="13" max="13" width="16.7109375" customWidth="1"/>
     <col min="14" max="14" width="25.28515625" customWidth="1"/>
     <col min="15" max="15" width="37.7109375" customWidth="1"/>
@@ -504,10 +504,10 @@
         <v>2</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>3</v>
@@ -522,22 +522,22 @@
         <v>5</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
added address 2 field
</commit_message>
<xml_diff>
--- a/saibabacharityreceiptor/template.xlsx
+++ b/saibabacharityreceiptor/template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Address</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Issued Date(mm/dd/yyyy)</t>
+  </si>
+  <si>
+    <t>Address2</t>
   </si>
 </sst>
 </file>
@@ -441,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -452,27 +455,27 @@
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
     <col min="3" max="3" width="6" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" customWidth="1"/>
-    <col min="6" max="7" width="6.42578125" customWidth="1"/>
-    <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="6.28515625" customWidth="1"/>
-    <col min="10" max="10" width="8.28515625" customWidth="1"/>
-    <col min="11" max="11" width="25.5703125" customWidth="1"/>
-    <col min="12" max="12" width="21" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" customWidth="1"/>
-    <col min="14" max="14" width="25.28515625" customWidth="1"/>
-    <col min="15" max="15" width="37.7109375" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" customWidth="1"/>
-    <col min="17" max="17" width="10.28515625" customWidth="1"/>
-    <col min="18" max="18" width="7.28515625" customWidth="1"/>
-    <col min="19" max="19" width="12.42578125" customWidth="1"/>
-    <col min="20" max="22" width="12.85546875" customWidth="1"/>
-    <col min="23" max="23" width="17.140625" customWidth="1"/>
-    <col min="24" max="24" width="13.5703125" customWidth="1"/>
+    <col min="4" max="5" width="10.28515625" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="7" max="8" width="6.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" customWidth="1"/>
+    <col min="12" max="12" width="25.5703125" customWidth="1"/>
+    <col min="13" max="13" width="21" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" customWidth="1"/>
+    <col min="15" max="15" width="25.28515625" customWidth="1"/>
+    <col min="16" max="16" width="37.7109375" customWidth="1"/>
+    <col min="17" max="17" width="17.28515625" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" customWidth="1"/>
+    <col min="19" max="19" width="7.28515625" customWidth="1"/>
+    <col min="20" max="20" width="12.42578125" customWidth="1"/>
+    <col min="21" max="23" width="12.85546875" customWidth="1"/>
+    <col min="24" max="24" width="17.140625" customWidth="1"/>
+    <col min="25" max="25" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1">
+    <row r="1" spans="1:25" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -489,65 +492,68 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
-      <c r="I2" s="2"/>
+    <row r="2" spans="1:25">
+      <c r="J2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>